<commit_message>
Now the program can iterate through all worksheets in an excel document, get the name of each worksheet and the number of rows and columns that the worksheet has data in.
</commit_message>
<xml_diff>
--- a/TestWorkbook.xlsx
+++ b/TestWorkbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\source\repos\ExcelReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F0706E9-0C57-4663-B15A-C55D8CC7D08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6BEEC5-11C7-4978-B00F-16E872C1B5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{8F24163C-8AC2-4BEA-80F1-B654281B7436}"/>
   </bookViews>
@@ -34,9 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A901D3B3-FCA8-45DE-9706-86C85937436D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,6 +404,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
There is now a column model which all of that columns data will be read into a list variable. It also will contain the Table name and column name. This should allow creation of the database column much easier.
</commit_message>
<xml_diff>
--- a/TestWorkbook.xlsx
+++ b/TestWorkbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\source\repos\ExcelReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6BEEC5-11C7-4978-B00F-16E872C1B5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B2410B-107C-4336-91F2-847423DF2510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{8F24163C-8AC2-4BEA-80F1-B654281B7436}"/>
   </bookViews>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>test</t>
   </si>
   <si>
     <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
   </si>
 </sst>
 </file>
@@ -393,15 +396,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A901D3B3-FCA8-45DE-9706-86C85937436D}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update to the workbook
</commit_message>
<xml_diff>
--- a/TestWorkbook.xlsx
+++ b/TestWorkbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\source\repos\ExcelReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6BEEC5-11C7-4978-B00F-16E872C1B5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B2410B-107C-4336-91F2-847423DF2510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{8F24163C-8AC2-4BEA-80F1-B654281B7436}"/>
   </bookViews>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>test</t>
   </si>
   <si>
     <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
   </si>
 </sst>
 </file>
@@ -393,15 +396,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A901D3B3-FCA8-45DE-9706-86C85937436D}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>